<commit_message>
added sector details; work at home 05-18-2016
</commit_message>
<xml_diff>
--- a/wa-esd-NonFarm-Industry-05132016.xlsx
+++ b/wa-esd-NonFarm-Industry-05132016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="23520" windowHeight="9735"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -501,12 +501,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,7 +725,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -760,7 +759,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -936,14 +934,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B70" sqref="B3:B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.7109375" bestFit="1" customWidth="1"/>
@@ -955,7 +953,7 @@
     <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -979,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1010,7 +1008,7 @@
         <v>88400</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1041,7 +1039,7 @@
         <v>56200</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1072,7 +1070,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1105,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1148,7 +1146,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1183,7 +1181,7 @@
         <v>35300</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1217,7 +1215,7 @@
         <v>49200</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1255,7 +1253,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1296,7 +1294,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1327,7 +1325,7 @@
         <v>7100</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1361,7 +1359,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1396,7 +1394,7 @@
         <v>32200</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1427,7 +1425,7 @@
         <v>18900</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1458,7 +1456,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1489,7 +1487,7 @@
         <v>11200</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1514,7 +1512,7 @@
         <v>13700</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1536,7 +1534,7 @@
       </c>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1561,7 +1559,7 @@
       </c>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1589,7 +1587,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1614,7 +1612,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1642,7 +1640,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -1667,7 +1665,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1692,7 +1690,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1717,7 +1715,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1742,7 +1740,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -1763,13 +1761,14 @@
         <v>59700</v>
       </c>
       <c r="H28" s="17">
-        <v>59700</v>
+        <f>G28-G31-G33</f>
+        <v>35700</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
@@ -1791,7 +1790,7 @@
       </c>
       <c r="H29" s="16"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -1813,7 +1812,7 @@
       </c>
       <c r="H30" s="16"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
@@ -1827,15 +1826,18 @@
       <c r="E31" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="13" t="s">
         <v>133</v>
       </c>
       <c r="G31" s="16">
         <v>3700</v>
       </c>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H31" s="16">
+        <f>G31+G33</f>
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1857,7 +1859,7 @@
       </c>
       <c r="H32" s="16"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
@@ -1879,7 +1881,7 @@
       </c>
       <c r="H33" s="16"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -1891,7 +1893,7 @@
       </c>
       <c r="D34" s="19"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
@@ -1903,7 +1905,7 @@
       </c>
       <c r="D35" s="19"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
@@ -1918,7 +1920,7 @@
         <v>84700</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
@@ -1930,7 +1932,7 @@
       </c>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
@@ -1942,7 +1944,7 @@
       </c>
       <c r="D38" s="19"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>74</v>
       </c>
@@ -1954,7 +1956,7 @@
       </c>
       <c r="D39" s="19"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
@@ -1966,7 +1968,7 @@
       </c>
       <c r="D40" s="19"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>78</v>
       </c>
@@ -1978,7 +1980,7 @@
       </c>
       <c r="D41" s="19"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -1990,7 +1992,7 @@
       </c>
       <c r="D42" s="19"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
@@ -2002,7 +2004,7 @@
       </c>
       <c r="D43" s="19"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
@@ -2014,7 +2016,7 @@
       </c>
       <c r="D44" s="19"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -2026,7 +2028,7 @@
       </c>
       <c r="D45" s="19"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
@@ -2038,7 +2040,7 @@
       </c>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
@@ -2050,7 +2052,7 @@
       </c>
       <c r="D47" s="19"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -2062,7 +2064,7 @@
       </c>
       <c r="D48" s="19"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -2074,7 +2076,7 @@
       </c>
       <c r="D49" s="19"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>96</v>
       </c>
@@ -2086,7 +2088,7 @@
       </c>
       <c r="D50" s="19"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -2098,7 +2100,7 @@
       </c>
       <c r="D51" s="19"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
@@ -2110,7 +2112,7 @@
       </c>
       <c r="D52" s="19"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>102</v>
       </c>
@@ -2122,7 +2124,7 @@
       </c>
       <c r="D53" s="19"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
@@ -2134,7 +2136,7 @@
       </c>
       <c r="D54" s="19"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>106</v>
       </c>
@@ -2146,7 +2148,7 @@
       </c>
       <c r="D55" s="19"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
@@ -2158,7 +2160,7 @@
       </c>
       <c r="D56" s="19"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>110</v>
       </c>
@@ -2170,7 +2172,7 @@
       </c>
       <c r="D57" s="19"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>112</v>
       </c>
@@ -2182,7 +2184,7 @@
       </c>
       <c r="D58" s="19"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>114</v>
       </c>
@@ -2194,7 +2196,7 @@
       </c>
       <c r="D59" s="19"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
         <v>116</v>
       </c>
@@ -2206,7 +2208,7 @@
       </c>
       <c r="D60" s="19"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>118</v>
       </c>
@@ -2218,7 +2220,7 @@
       </c>
       <c r="D61" s="19"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>120</v>
       </c>
@@ -2230,7 +2232,7 @@
       </c>
       <c r="D62" s="19"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>122</v>
       </c>
@@ -2242,7 +2244,7 @@
       </c>
       <c r="D63" s="19"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>124</v>
       </c>
@@ -2254,7 +2256,7 @@
       </c>
       <c r="D64" s="19"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
         <v>126</v>
       </c>
@@ -2265,11 +2267,11 @@
         <v>216500</v>
       </c>
       <c r="D65" s="22">
-        <f>C65</f>
-        <v>216500</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <f>C65-C68-C70</f>
+        <v>112300</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
         <v>128</v>
       </c>
@@ -2281,7 +2283,7 @@
       </c>
       <c r="D66" s="19"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
         <v>130</v>
       </c>
@@ -2293,19 +2295,22 @@
       </c>
       <c r="D67" s="19"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="13" t="s">
         <v>133</v>
       </c>
       <c r="C68" s="22">
         <v>48300</v>
       </c>
-      <c r="D68" s="19"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="22">
+        <f>C68+C70</f>
+        <v>104200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
         <v>134</v>
       </c>
@@ -2317,7 +2322,7 @@
       </c>
       <c r="D69" s="19"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
         <v>136</v>
       </c>
@@ -2335,24 +2340,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
work at office 05-23-2016
</commit_message>
<xml_diff>
--- a/wa-esd-NonFarm-Industry-05132016.xlsx
+++ b/wa-esd-NonFarm-Industry-05132016.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="23520" windowHeight="9735"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -501,12 +501,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy:mm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,6 +725,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -759,6 +760,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -934,14 +936,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B70" sqref="B3:B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.7109375" bestFit="1" customWidth="1"/>
@@ -953,7 +955,7 @@
     <col min="10" max="10" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -977,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1008,7 +1010,7 @@
         <v>88400</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1039,7 +1041,7 @@
         <v>56200</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1070,7 +1072,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1105,7 +1107,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1146,7 +1148,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1181,7 +1183,7 @@
         <v>35300</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1215,7 +1217,7 @@
         <v>49200</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1253,7 +1255,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1294,7 +1296,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1325,7 +1327,7 @@
         <v>7100</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1359,7 +1361,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1394,7 +1396,7 @@
         <v>32200</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1425,7 +1427,7 @@
         <v>18900</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1456,7 +1458,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1487,7 +1489,7 @@
         <v>11200</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1512,7 +1514,7 @@
         <v>13700</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -1534,7 +1536,7 @@
       </c>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1559,7 +1561,7 @@
       </c>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1587,7 +1589,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1612,7 +1614,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1640,7 +1642,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -1665,7 +1667,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1690,7 +1692,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1715,7 +1717,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
@@ -1740,7 +1742,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>52</v>
       </c>
@@ -1768,7 +1770,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>54</v>
       </c>
@@ -1790,7 +1792,7 @@
       </c>
       <c r="H29" s="16"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -1812,7 +1814,7 @@
       </c>
       <c r="H30" s="16"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
@@ -1837,7 +1839,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1859,7 +1861,7 @@
       </c>
       <c r="H32" s="16"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
@@ -1881,7 +1883,7 @@
       </c>
       <c r="H33" s="16"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>64</v>
       </c>
@@ -1893,7 +1895,7 @@
       </c>
       <c r="D34" s="19"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
@@ -1905,7 +1907,7 @@
       </c>
       <c r="D35" s="19"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>68</v>
       </c>
@@ -1920,7 +1922,7 @@
         <v>84700</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
@@ -1932,7 +1934,7 @@
       </c>
       <c r="D37" s="19"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>72</v>
       </c>
@@ -1944,7 +1946,7 @@
       </c>
       <c r="D38" s="19"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>74</v>
       </c>
@@ -1956,7 +1958,7 @@
       </c>
       <c r="D39" s="19"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>76</v>
       </c>
@@ -1968,7 +1970,7 @@
       </c>
       <c r="D40" s="19"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>78</v>
       </c>
@@ -1980,7 +1982,7 @@
       </c>
       <c r="D41" s="19"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -1992,7 +1994,7 @@
       </c>
       <c r="D42" s="19"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
@@ -2004,7 +2006,7 @@
       </c>
       <c r="D43" s="19"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
@@ -2016,7 +2018,7 @@
       </c>
       <c r="D44" s="19"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
@@ -2028,7 +2030,7 @@
       </c>
       <c r="D45" s="19"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>88</v>
       </c>
@@ -2040,7 +2042,7 @@
       </c>
       <c r="D46" s="19"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>90</v>
       </c>
@@ -2052,7 +2054,7 @@
       </c>
       <c r="D47" s="19"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>92</v>
       </c>
@@ -2064,7 +2066,7 @@
       </c>
       <c r="D48" s="19"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
@@ -2076,7 +2078,7 @@
       </c>
       <c r="D49" s="19"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>96</v>
       </c>
@@ -2088,7 +2090,7 @@
       </c>
       <c r="D50" s="19"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -2100,7 +2102,7 @@
       </c>
       <c r="D51" s="19"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
@@ -2112,7 +2114,7 @@
       </c>
       <c r="D52" s="19"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>102</v>
       </c>
@@ -2124,7 +2126,7 @@
       </c>
       <c r="D53" s="19"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
@@ -2136,7 +2138,7 @@
       </c>
       <c r="D54" s="19"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>106</v>
       </c>
@@ -2148,7 +2150,7 @@
       </c>
       <c r="D55" s="19"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
@@ -2160,7 +2162,7 @@
       </c>
       <c r="D56" s="19"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>110</v>
       </c>
@@ -2172,7 +2174,7 @@
       </c>
       <c r="D57" s="19"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>112</v>
       </c>
@@ -2184,7 +2186,7 @@
       </c>
       <c r="D58" s="19"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>114</v>
       </c>
@@ -2196,7 +2198,7 @@
       </c>
       <c r="D59" s="19"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>116</v>
       </c>
@@ -2208,7 +2210,7 @@
       </c>
       <c r="D60" s="19"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>118</v>
       </c>
@@ -2220,7 +2222,7 @@
       </c>
       <c r="D61" s="19"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>120</v>
       </c>
@@ -2232,7 +2234,7 @@
       </c>
       <c r="D62" s="19"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>122</v>
       </c>
@@ -2244,7 +2246,7 @@
       </c>
       <c r="D63" s="19"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>124</v>
       </c>
@@ -2256,7 +2258,7 @@
       </c>
       <c r="D64" s="19"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>126</v>
       </c>
@@ -2271,7 +2273,7 @@
         <v>112300</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>128</v>
       </c>
@@ -2283,7 +2285,7 @@
       </c>
       <c r="D66" s="19"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>130</v>
       </c>
@@ -2295,7 +2297,7 @@
       </c>
       <c r="D67" s="19"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>132</v>
       </c>
@@ -2310,7 +2312,7 @@
         <v>104200</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>134</v>
       </c>
@@ -2322,7 +2324,7 @@
       </c>
       <c r="D69" s="19"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>136</v>
       </c>
@@ -2340,24 +2342,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>